<commit_message>
+ add panel legend on figures
</commit_message>
<xml_diff>
--- a/rawdata/colnames12_v2.xlsx
+++ b/rawdata/colnames12_v2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2940BB-1A8F-4806-8B75-AB3F1D36F522}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5B3A2A-F1D5-4F10-91E6-42806FF5DFD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,15 +262,6 @@
     <t>Color_bar22</t>
   </si>
   <si>
-    <t xml:space="preserve">Human </t>
-  </si>
-  <si>
-    <t>Ecosystem</t>
-  </si>
-  <si>
-    <t>Human</t>
-  </si>
-  <si>
     <t>Type_CA2</t>
   </si>
   <si>
@@ -281,6 +272,15 @@
   </si>
   <si>
     <t>#E1BC84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social justice </t>
+  </si>
+  <si>
+    <t>Social justice</t>
+  </si>
+  <si>
+    <t>Environmental justice</t>
   </si>
 </sst>
 </file>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,10 +666,10 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
@@ -767,7 +767,7 @@
         <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>11</v>
@@ -808,7 +808,7 @@
         <v>16</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>16</v>
@@ -1109,7 +1109,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>16</v>
@@ -1179,7 +1179,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>16</v>
@@ -1216,7 +1216,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>16</v>
@@ -1257,7 +1257,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>16</v>
@@ -1269,7 +1269,7 @@
         <v>16</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>16</v>
@@ -1298,7 +1298,7 @@
         <v>16</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>16</v>
@@ -1310,7 +1310,7 @@
         <v>16</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>16</v>
@@ -1339,7 +1339,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>16</v>
@@ -1351,7 +1351,7 @@
         <v>16</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>16</v>
@@ -1380,7 +1380,7 @@
         <v>16</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>16</v>
@@ -1392,7 +1392,7 @@
         <v>16</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>16</v>
@@ -1421,7 +1421,7 @@
         <v>16</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>11</v>
@@ -1433,7 +1433,7 @@
         <v>16</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>11</v>
@@ -1462,7 +1462,7 @@
         <v>16</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>11</v>
@@ -1474,7 +1474,7 @@
         <v>16</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>11</v>
@@ -1499,7 +1499,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>16</v>
@@ -1511,7 +1511,7 @@
         <v>35</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>16</v>
@@ -1528,10 +1528,10 @@
         <v>0.42425585799999999</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1544,10 +1544,10 @@
         <v>35</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1561,10 +1561,10 @@
         <v>0.42425585799999999</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1577,10 +1577,10 @@
         <v>35</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -1594,10 +1594,10 @@
         <v>0.42425585799999999</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1610,10 +1610,10 @@
         <v>35</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -1627,10 +1627,10 @@
         <v>0.42425585799999999</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1643,10 +1643,10 @@
         <v>35</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -1734,7 +1734,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>16</v>
@@ -1746,7 +1746,7 @@
         <v>35</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>16</v>
@@ -1862,10 +1862,10 @@
         <v>0.10191048</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1878,10 +1878,10 @@
         <v>35</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -1895,10 +1895,10 @@
         <v>0.10191048</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1911,10 +1911,10 @@
         <v>35</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -1928,10 +1928,10 @@
         <v>0.10191048</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1944,10 +1944,10 @@
         <v>35</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -1965,7 +1965,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>16</v>
@@ -1977,7 +1977,7 @@
         <v>35</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>16</v>
@@ -2002,7 +2002,7 @@
         <v>16</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>16</v>
@@ -2014,7 +2014,7 @@
         <v>16</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>16</v>
@@ -2039,7 +2039,7 @@
         <v>11</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>11</v>
@@ -2051,7 +2051,7 @@
         <v>11</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>11</v>
@@ -2072,7 +2072,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>16</v>
@@ -2084,7 +2084,7 @@
         <v>35</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>16</v>
@@ -2109,7 +2109,7 @@
         <v>16</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>11</v>
@@ -2121,7 +2121,7 @@
         <v>16</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>11</v>
@@ -2146,7 +2146,7 @@
         <v>16</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>11</v>
@@ -2158,7 +2158,7 @@
         <v>16</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>11</v>
@@ -2183,7 +2183,7 @@
         <v>11</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>11</v>
@@ -2195,7 +2195,7 @@
         <v>11</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>11</v>
@@ -2220,7 +2220,7 @@
         <v>11</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>11</v>
@@ -2232,7 +2232,7 @@
         <v>11</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>11</v>
@@ -2257,7 +2257,7 @@
         <v>11</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>11</v>
@@ -2269,7 +2269,7 @@
         <v>11</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M46" s="2" t="s">
         <v>11</v>
@@ -2290,7 +2290,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>11</v>
@@ -2302,7 +2302,7 @@
         <v>35</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M47" s="2" t="s">
         <v>11</v>
@@ -2327,7 +2327,7 @@
         <v>11</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>11</v>
@@ -2339,7 +2339,7 @@
         <v>11</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M48" s="2" t="s">
         <v>11</v>
@@ -2360,7 +2360,7 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>11</v>
@@ -2372,7 +2372,7 @@
         <v>35</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>11</v>
@@ -2393,7 +2393,7 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>11</v>
@@ -2405,7 +2405,7 @@
         <v>35</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M50" s="2" t="s">
         <v>11</v>
@@ -2430,7 +2430,7 @@
         <v>35</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>11</v>
@@ -2442,7 +2442,7 @@
         <v>35</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M51" s="2" t="s">
         <v>11</v>
@@ -2463,7 +2463,7 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>11</v>
@@ -2475,7 +2475,7 @@
         <v>35</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M52" s="2" t="s">
         <v>11</v>
@@ -2500,7 +2500,7 @@
         <v>16</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>11</v>
@@ -2512,7 +2512,7 @@
         <v>16</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M53" s="2" t="s">
         <v>11</v>
@@ -2533,7 +2533,7 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>11</v>
@@ -2545,7 +2545,7 @@
         <v>35</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M54" s="2" t="s">
         <v>11</v>
@@ -2570,7 +2570,7 @@
         <v>11</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>11</v>
@@ -2582,7 +2582,7 @@
         <v>11</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M55" s="2" t="s">
         <v>11</v>
@@ -2607,7 +2607,7 @@
         <v>11</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>11</v>
@@ -2619,7 +2619,7 @@
         <v>11</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M56" s="2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
change legend on figure3
</commit_message>
<xml_diff>
--- a/rawdata/colnames12_v2.xlsx
+++ b/rawdata/colnames12_v2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5B3A2A-F1D5-4F10-91E6-42806FF5DFD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE9EE04-543C-4C37-B097-890BF45BF74D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>